<commit_message>
Adding example. Baby classic
Former-commit-id: 0723aeeac9352b4355c405fbe1c56888d6ffb8f6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="23540"/>
   </bookViews>
   <sheets>
     <sheet name="BabyDragons" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>[sku]</t>
   </si>
@@ -53,9 +53,6 @@
     <t>[tidDesc]</t>
   </si>
   <si>
-    <t>food</t>
-  </si>
-  <si>
     <t>[category]</t>
   </si>
   <si>
@@ -87,12 +84,6 @@
   </si>
   <si>
     <t>coins_better</t>
-  </si>
-  <si>
-    <t>score_better</t>
-  </si>
-  <si>
-    <t>baby_0</t>
   </si>
   <si>
     <t>baby_1</t>
@@ -268,6 +259,30 @@
       </rPr>
       <t xml:space="preserve"> firsts Flying pigs killed (with a Baby D. equipped) player doesn't get an 'extra' Gem, we will set prob. to 100% next time player kills a Flying pig, after that, prob. will be what was before. We need this value to 'show' player it is true they can get extra Gems and encourage them to get more Baby D.</t>
     </r>
+  </si>
+  <si>
+    <t>baby_classic</t>
+  </si>
+  <si>
+    <t>TID_BABY_DRAGON_UNLOCK</t>
+  </si>
+  <si>
+    <t>PF_BabyClassic</t>
+  </si>
+  <si>
+    <t>PF_BabyClassicMenu</t>
+  </si>
+  <si>
+    <t>dragon_classic</t>
+  </si>
+  <si>
+    <t>TID_BABY_CLASSIC_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_CLASSIC_DESC</t>
+  </si>
+  <si>
+    <t>hp</t>
   </si>
 </sst>
 </file>
@@ -679,6 +694,31 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -694,19 +734,20 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -729,23 +770,22 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -754,6 +794,36 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -894,6 +964,84 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1428,42 +1576,42 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1497,139 +1645,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -1646,48 +1661,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V7" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" headerRowBorderDxfId="25" tableBorderDxfId="26" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B4:V7"/>
   <sortState ref="B5:T77">
     <sortCondition ref="D4:D77"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="23"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="22"/>
-    <tableColumn id="3" name="[rarity]" dataDxfId="21"/>
-    <tableColumn id="6" name="[category]" dataDxfId="20"/>
-    <tableColumn id="7" name="[order]" dataDxfId="19"/>
-    <tableColumn id="13" name="[startingPool]" dataDxfId="18"/>
-    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="17"/>
-    <tableColumn id="16" name="[hidden]" dataDxfId="16"/>
-    <tableColumn id="15" name="[notInGatcha]" dataDxfId="15"/>
-    <tableColumn id="18" name="[associatedSeason]" dataDxfId="14"/>
-    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="13"/>
-    <tableColumn id="8" name="[gamePrefab]" dataDxfId="12"/>
-    <tableColumn id="9" name="[menuPrefab]" dataDxfId="11"/>
-    <tableColumn id="11" name="[icon]" dataDxfId="10"/>
-    <tableColumn id="4" name="[powerup]" dataDxfId="9"/>
-    <tableColumn id="20" name="[statPower]" dataDxfId="4"/>
-    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="8"/>
-    <tableColumn id="10" name="[tidDesc]" dataDxfId="7"/>
-    <tableColumn id="12" name="id" dataDxfId="6"/>
-    <tableColumn id="17" name="[trackingName]" dataDxfId="5"/>
+    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="29"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
+    <tableColumn id="3" name="[rarity]" dataDxfId="27"/>
+    <tableColumn id="6" name="[category]" dataDxfId="26"/>
+    <tableColumn id="7" name="[order]" dataDxfId="25"/>
+    <tableColumn id="13" name="[startingPool]" dataDxfId="24"/>
+    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="23"/>
+    <tableColumn id="16" name="[hidden]" dataDxfId="22"/>
+    <tableColumn id="15" name="[notInGatcha]" dataDxfId="21"/>
+    <tableColumn id="18" name="[associatedSeason]" dataDxfId="20"/>
+    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="19"/>
+    <tableColumn id="8" name="[gamePrefab]" dataDxfId="18"/>
+    <tableColumn id="9" name="[menuPrefab]" dataDxfId="17"/>
+    <tableColumn id="11" name="[icon]" dataDxfId="16"/>
+    <tableColumn id="4" name="[powerup]" dataDxfId="15"/>
+    <tableColumn id="20" name="[statPower]" dataDxfId="14"/>
+    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="13"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="12"/>
+    <tableColumn id="10" name="[tidDesc]" dataDxfId="11"/>
+    <tableColumn id="12" name="id" dataDxfId="10"/>
+    <tableColumn id="17" name="[trackingName]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B12:G13" totalsRowShown="0" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B12:G13" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B12:G13"/>
   <sortState ref="B95:F101">
     <sortCondition ref="D77:D84"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="31"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
-    <tableColumn id="3" name="[baseProbability]" dataDxfId="29"/>
+    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="5"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
+    <tableColumn id="3" name="[baseProbability]" dataDxfId="3"/>
     <tableColumn id="4" name="[extraProbability]" dataDxfId="2"/>
     <tableColumn id="5" name="[extraGems]" dataDxfId="1"/>
     <tableColumn id="6" name="[firstSucceed]" dataDxfId="0"/>
@@ -1964,37 +1979,37 @@
   </sheetPr>
   <dimension ref="B1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.42578125" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" customWidth="1"/>
+    <col min="8" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.453125" customWidth="1"/>
+    <col min="13" max="13" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="29.81640625" customWidth="1"/>
     <col min="19" max="19" width="23" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:22" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2009,20 +2024,20 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="23"/>
       <c r="P3" s="26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="121.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" ht="119" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -2031,34 +2046,34 @@
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>1</v>
@@ -2067,10 +2082,10 @@
         <v>7</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>4</v>
@@ -2082,24 +2097,24 @@
         <v>3</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>25</v>
-      </c>
       <c r="E5" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G5" s="18" t="b">
         <v>0</v>
@@ -2114,34 +2129,52 @@
         <v>0</v>
       </c>
       <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="L5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="P5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="U5" s="11">
         <v>0</v>
       </c>
-      <c r="V5" s="18"/>
+      <c r="V5" s="18" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="18">
         <v>1</v>
@@ -2163,9 +2196,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="P6" s="15"/>
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
       <c r="S6" s="11"/>
@@ -2175,18 +2206,18 @@
       </c>
       <c r="V6" s="18"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="18">
         <v>2</v>
@@ -2208,9 +2239,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
-      <c r="P7" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="P7" s="15"/>
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
       <c r="S7" s="11"/>
@@ -2220,10 +2249,10 @@
       </c>
       <c r="V7" s="18"/>
     </row>
-    <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:22" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2238,36 +2267,36 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:22" ht="137.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" ht="134" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" s="13">
         <v>10</v>
@@ -2282,29 +2311,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C19" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="28" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="28" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a column to specify the sharedpower
Former-commit-id: d394dc59eed216c76dd376ff6b02e7f7aa44e83e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
   </bookViews>
   <sheets>
     <sheet name="BabyDragons" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>[sku]</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>hp</t>
+  </si>
+  <si>
+    <t>[sharedPower]</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,46 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1661,51 +1703,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
-  <autoFilter ref="B4:V7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:W7" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+  <autoFilter ref="B4:W7"/>
   <sortState ref="B5:T77">
     <sortCondition ref="D4:D77"/>
   </sortState>
-  <tableColumns count="21">
-    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="3" name="[rarity]" dataDxfId="27"/>
-    <tableColumn id="6" name="[category]" dataDxfId="26"/>
-    <tableColumn id="7" name="[order]" dataDxfId="25"/>
-    <tableColumn id="13" name="[startingPool]" dataDxfId="24"/>
-    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="23"/>
-    <tableColumn id="16" name="[hidden]" dataDxfId="22"/>
-    <tableColumn id="15" name="[notInGatcha]" dataDxfId="21"/>
-    <tableColumn id="18" name="[associatedSeason]" dataDxfId="20"/>
-    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="19"/>
-    <tableColumn id="8" name="[gamePrefab]" dataDxfId="18"/>
-    <tableColumn id="9" name="[menuPrefab]" dataDxfId="17"/>
-    <tableColumn id="11" name="[icon]" dataDxfId="16"/>
-    <tableColumn id="4" name="[powerup]" dataDxfId="15"/>
-    <tableColumn id="20" name="[statPower]" dataDxfId="14"/>
-    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="13"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="12"/>
-    <tableColumn id="10" name="[tidDesc]" dataDxfId="11"/>
-    <tableColumn id="12" name="id" dataDxfId="10"/>
-    <tableColumn id="17" name="[trackingName]" dataDxfId="9"/>
+  <tableColumns count="22">
+    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[rarity]" dataDxfId="28"/>
+    <tableColumn id="6" name="[category]" dataDxfId="27"/>
+    <tableColumn id="7" name="[order]" dataDxfId="26"/>
+    <tableColumn id="13" name="[startingPool]" dataDxfId="25"/>
+    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="24"/>
+    <tableColumn id="16" name="[hidden]" dataDxfId="23"/>
+    <tableColumn id="15" name="[notInGatcha]" dataDxfId="22"/>
+    <tableColumn id="18" name="[associatedSeason]" dataDxfId="21"/>
+    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="20"/>
+    <tableColumn id="8" name="[gamePrefab]" dataDxfId="19"/>
+    <tableColumn id="9" name="[menuPrefab]" dataDxfId="18"/>
+    <tableColumn id="11" name="[icon]" dataDxfId="17"/>
+    <tableColumn id="4" name="[powerup]" dataDxfId="16"/>
+    <tableColumn id="20" name="[statPower]" dataDxfId="15"/>
+    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="14"/>
+    <tableColumn id="22" name="[sharedPower]" dataDxfId="0"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="13"/>
+    <tableColumn id="10" name="[tidDesc]" dataDxfId="12"/>
+    <tableColumn id="12" name="id" dataDxfId="11"/>
+    <tableColumn id="17" name="[trackingName]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B12:G13" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B12:G13" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B12:G13"/>
   <sortState ref="B95:F101">
     <sortCondition ref="D77:D84"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="5"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
-    <tableColumn id="3" name="[baseProbability]" dataDxfId="3"/>
-    <tableColumn id="4" name="[extraProbability]" dataDxfId="2"/>
-    <tableColumn id="5" name="[extraGems]" dataDxfId="1"/>
-    <tableColumn id="6" name="[firstSucceed]" dataDxfId="0"/>
+    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="6"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="3" name="[baseProbability]" dataDxfId="4"/>
+    <tableColumn id="4" name="[extraProbability]" dataDxfId="3"/>
+    <tableColumn id="5" name="[extraGems]" dataDxfId="2"/>
+    <tableColumn id="6" name="[firstSucceed]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1977,37 +2020,37 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:V22"/>
+  <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.453125" customWidth="1"/>
-    <col min="8" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.453125" customWidth="1"/>
-    <col min="13" max="13" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="29.81640625" customWidth="1"/>
-    <col min="19" max="19" width="23" customWidth="1"/>
-    <col min="20" max="20" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.42578125" customWidth="1"/>
+    <col min="13" max="13" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="29.85546875" customWidth="1"/>
+    <col min="20" max="20" width="23" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:22" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
@@ -2024,7 +2067,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="23"/>
@@ -2035,7 +2078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="119" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:23" ht="121.5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
@@ -2087,20 +2130,23 @@
       <c r="R4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="U4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="V4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
@@ -2150,20 +2196,23 @@
       <c r="R5" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="S5" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="U5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="U5" s="11">
+      <c r="V5" s="11">
         <v>0</v>
       </c>
-      <c r="V5" s="18" t="s">
+      <c r="W5" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
@@ -2199,14 +2248,17 @@
       <c r="P6" s="15"/>
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
-      <c r="S6" s="11"/>
+      <c r="S6" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="T6" s="11"/>
-      <c r="U6" s="16">
+      <c r="U6" s="11"/>
+      <c r="V6" s="16">
         <v>1</v>
       </c>
-      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
@@ -2242,15 +2294,18 @@
       <c r="P7" s="15"/>
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="11">
+      <c r="S7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7" s="11"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="11">
         <v>2</v>
       </c>
-      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
     </row>
-    <row r="9" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:22" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -2267,11 +2322,11 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:22" ht="134" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:23" ht="137.25" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
@@ -2291,7 +2346,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
@@ -2311,27 +2366,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" s="28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" s="28" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Adding specific powerups for Baby dragons
Former-commit-id: e4a1ae842cad4c2decc22cd421de5544674fb09c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="23540"/>
   </bookViews>
   <sheets>
     <sheet name="BabyDragons" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>[sku]</t>
   </si>
@@ -84,12 +84,6 @@
   </si>
   <si>
     <t>coins_better</t>
-  </si>
-  <si>
-    <t>baby_1</t>
-  </si>
-  <si>
-    <t>baby_2</t>
   </si>
   <si>
     <t>baby</t>
@@ -282,10 +276,49 @@
     <t>TID_BABY_CLASSIC_DESC</t>
   </si>
   <si>
-    <t>hp</t>
-  </si>
-  <si>
     <t>[sharedPower]</t>
+  </si>
+  <si>
+    <t>baby_crocodile</t>
+  </si>
+  <si>
+    <t>baby_titan</t>
+  </si>
+  <si>
+    <t>PF_BabyCrocodile</t>
+  </si>
+  <si>
+    <t>PF_BabyTitan</t>
+  </si>
+  <si>
+    <t>PF_BabyCrocodileMenu</t>
+  </si>
+  <si>
+    <t>PF_BabyTitanMenu</t>
+  </si>
+  <si>
+    <t>dragon_crocodile</t>
+  </si>
+  <si>
+    <t>dragon_titan</t>
+  </si>
+  <si>
+    <t>TID_BABY_CROCODILE_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_TITAN_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_TITAN_DESC</t>
+  </si>
+  <si>
+    <t>baby_fury_duration</t>
+  </si>
+  <si>
+    <t>baby_lower_damage_dragon</t>
+  </si>
+  <si>
+    <t>baby_prey_hp_boost_humans</t>
   </si>
 </sst>
 </file>
@@ -646,45 +679,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1006,6 +1000,45 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1726,29 +1759,29 @@
     <tableColumn id="4" name="[powerup]" dataDxfId="16"/>
     <tableColumn id="20" name="[statPower]" dataDxfId="15"/>
     <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="14"/>
-    <tableColumn id="22" name="[sharedPower]" dataDxfId="0"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="13"/>
-    <tableColumn id="10" name="[tidDesc]" dataDxfId="12"/>
-    <tableColumn id="12" name="id" dataDxfId="11"/>
-    <tableColumn id="17" name="[trackingName]" dataDxfId="10"/>
+    <tableColumn id="22" name="[sharedPower]" dataDxfId="13"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="12"/>
+    <tableColumn id="10" name="[tidDesc]" dataDxfId="11"/>
+    <tableColumn id="12" name="id" dataDxfId="10"/>
+    <tableColumn id="17" name="[trackingName]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B12:G13" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B12:G13" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B12:G13"/>
   <sortState ref="B95:F101">
     <sortCondition ref="D77:D84"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="6"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="3" name="[baseProbability]" dataDxfId="4"/>
-    <tableColumn id="4" name="[extraProbability]" dataDxfId="3"/>
-    <tableColumn id="5" name="[extraGems]" dataDxfId="2"/>
-    <tableColumn id="6" name="[firstSucceed]" dataDxfId="1"/>
+    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="5"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
+    <tableColumn id="3" name="[baseProbability]" dataDxfId="3"/>
+    <tableColumn id="4" name="[extraProbability]" dataDxfId="2"/>
+    <tableColumn id="5" name="[extraGems]" dataDxfId="1"/>
+    <tableColumn id="6" name="[firstSucceed]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2022,37 +2055,37 @@
   </sheetPr>
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.42578125" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" customWidth="1"/>
+    <col min="8" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.453125" customWidth="1"/>
+    <col min="13" max="13" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="29.81640625" customWidth="1"/>
     <col min="20" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2067,20 +2100,20 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="23"/>
       <c r="P3" s="26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:23" ht="121.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" ht="119" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -2125,13 +2158,13 @@
         <v>7</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S4" s="24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>4</v>
@@ -2146,21 +2179,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G5" s="18" t="b">
         <v>0</v>
@@ -2176,57 +2209,57 @@
       </c>
       <c r="K5" s="18"/>
       <c r="L5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="O5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="Q5" s="25" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="R5" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="S5" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="V5" s="11">
         <v>0</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F6" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="18" t="b">
         <v>1</v>
@@ -2241,38 +2274,58 @@
         <v>0</v>
       </c>
       <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
+      <c r="L6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="R6" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="S6" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="V6" s="16">
         <v>1</v>
       </c>
-      <c r="W6" s="18"/>
+      <c r="W6" s="18" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="18" t="b">
         <v>1</v>
@@ -2287,27 +2340,47 @@
         <v>0</v>
       </c>
       <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
+      <c r="L7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="S7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" s="11"/>
-      <c r="U7" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="V7" s="11">
         <v>2</v>
       </c>
-      <c r="W7" s="18"/>
+      <c r="W7" s="18" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="9" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2322,36 +2395,36 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:23" ht="137.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" ht="134" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="13">
         <v>10</v>
@@ -2366,29 +2439,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C19" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="28" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="28" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="28" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding powerups needed for Baby
Former-commit-id: b2df8df7f187650eac9da6fe73123d4494de2c8b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
   </bookViews>
   <sheets>
     <sheet name="BabyDragons" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>[sku]</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>[tidUnlockCondition]</t>
-  </si>
-  <si>
-    <t>coins_better</t>
   </si>
   <si>
     <t>baby</t>
@@ -319,6 +316,15 @@
   </si>
   <si>
     <t>baby_prey_hp_boost_humans</t>
+  </si>
+  <si>
+    <t>baby_transform_food</t>
+  </si>
+  <si>
+    <t>baby_phoenix_better</t>
+  </si>
+  <si>
+    <t>baby_kill_humanoid_burp</t>
   </si>
 </sst>
 </file>
@@ -2055,37 +2061,37 @@
   </sheetPr>
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.453125" customWidth="1"/>
-    <col min="8" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.453125" customWidth="1"/>
-    <col min="13" max="13" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="29.81640625" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.42578125" customWidth="1"/>
+    <col min="13" max="13" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="29.85546875" customWidth="1"/>
     <col min="20" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2100,20 +2106,20 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="23"/>
       <c r="P3" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="26" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="4" spans="2:23" ht="119" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:23" ht="121.5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -2158,13 +2164,13 @@
         <v>7</v>
       </c>
       <c r="Q4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="24" t="s">
-        <v>22</v>
-      </c>
       <c r="S4" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>4</v>
@@ -2179,18 +2185,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="18">
         <v>1</v>
@@ -2209,54 +2215,54 @@
       </c>
       <c r="K5" s="18"/>
       <c r="L5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="R5" s="25" t="s">
+      <c r="S5" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="S5" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="T5" s="11" t="s">
+      <c r="U5" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="V5" s="11">
         <v>0</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="18">
         <v>2</v>
@@ -2275,54 +2281,54 @@
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R6" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S6" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V6" s="16">
         <v>1</v>
       </c>
       <c r="W6" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="18">
         <v>3</v>
@@ -2341,46 +2347,46 @@
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R7" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S7" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="V7" s="11">
         <v>2</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2395,36 +2401,36 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:23" ht="134" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:23" ht="137.25" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="13">
         <v>10</v>
@@ -2439,29 +2445,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" s="28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C20" s="28" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C21" s="28" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="28" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C22" s="28" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final powerups and Baby D. tables (not exported xml yet)
Former-commit-id: 3e1bed5f9d5a47cf6f1acde74705affe56aad1b0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="116">
   <si>
     <t>[sku]</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>&lt;Definition&gt;</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
   <si>
     <t>[tidName]</t>
@@ -326,12 +323,174 @@
   <si>
     <t>baby_kill_humanoid_burp</t>
   </si>
+  <si>
+    <t>baby_jawfrey</t>
+  </si>
+  <si>
+    <t>baby_dark</t>
+  </si>
+  <si>
+    <t>baby_dino</t>
+  </si>
+  <si>
+    <t>baby_alien</t>
+  </si>
+  <si>
+    <t>baby_devil</t>
+  </si>
+  <si>
+    <t>baby_tony</t>
+  </si>
+  <si>
+    <t>baby_hedgehog</t>
+  </si>
+  <si>
+    <t>PF_BabyJawfrey</t>
+  </si>
+  <si>
+    <t>PF_BabyDark</t>
+  </si>
+  <si>
+    <t>PF_BabyDino</t>
+  </si>
+  <si>
+    <t>PF_BabyAlien</t>
+  </si>
+  <si>
+    <t>PF_BabyDevil</t>
+  </si>
+  <si>
+    <t>PF_BabyTony</t>
+  </si>
+  <si>
+    <t>PF_BabyHedgehog</t>
+  </si>
+  <si>
+    <t>PF_BabyJawfreyMenu</t>
+  </si>
+  <si>
+    <t>PF_BabyDarkMenu</t>
+  </si>
+  <si>
+    <t>PF_BabyDinoMenu</t>
+  </si>
+  <si>
+    <t>PF_BabyAlienMenu</t>
+  </si>
+  <si>
+    <t>PF_BabyDevilMenu</t>
+  </si>
+  <si>
+    <t>PF_BabyTonyMenu</t>
+  </si>
+  <si>
+    <t>PF_BabyHedgehogMenu</t>
+  </si>
+  <si>
+    <t>dragon_jawfrey</t>
+  </si>
+  <si>
+    <t>dragon_dark</t>
+  </si>
+  <si>
+    <t>dragon_dino</t>
+  </si>
+  <si>
+    <t>dragon_alien</t>
+  </si>
+  <si>
+    <t>dragon_devil</t>
+  </si>
+  <si>
+    <t>dragon_tony</t>
+  </si>
+  <si>
+    <t>dragon_hedgehog</t>
+  </si>
+  <si>
+    <t>TID_BABY_JAWFREY_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_DARK_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_DINO_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_ALIEN_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_DEVIL_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_TONY_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_HEDEGEHOG_NAME</t>
+  </si>
+  <si>
+    <t>TID_BABY_JAWFREY_DESC</t>
+  </si>
+  <si>
+    <t>TID_BABY_DARK_DESC</t>
+  </si>
+  <si>
+    <t>TID_BABY_DINO_DESC</t>
+  </si>
+  <si>
+    <t>TID_BABY_ALIEN_DESC</t>
+  </si>
+  <si>
+    <t>TID_BABY_DEVIL_DESC</t>
+  </si>
+  <si>
+    <t>TID_BABY_TONY_DESC</t>
+  </si>
+  <si>
+    <t>baby_speed</t>
+  </si>
+  <si>
+    <t>baby_magnet</t>
+  </si>
+  <si>
+    <t>baby_prey_hp_boost_dragon</t>
+  </si>
+  <si>
+    <t>baby_unlimited_boost</t>
+  </si>
+  <si>
+    <t>baby_food</t>
+  </si>
+  <si>
+    <t>baby_stun</t>
+  </si>
+  <si>
+    <t>baby_fireball</t>
+  </si>
+  <si>
+    <t>baby_more_xp</t>
+  </si>
+  <si>
+    <t>baby_sun</t>
+  </si>
+  <si>
+    <t>baby_boost</t>
+  </si>
+  <si>
+    <t>baby_drop_present</t>
+  </si>
+  <si>
+    <t>baby_score_better</t>
+  </si>
+  <si>
+    <t>baby_shoot_spikes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,6 +540,12 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -584,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -664,11 +829,68 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="35">
     <dxf>
       <font>
         <b val="0"/>
@@ -902,40 +1124,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1742,33 +1930,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:W7" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
-  <autoFilter ref="B4:W7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V14" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+  <autoFilter ref="B4:V14"/>
   <sortState ref="B5:T77">
     <sortCondition ref="D4:D77"/>
   </sortState>
-  <tableColumns count="22">
-    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="30"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[rarity]" dataDxfId="28"/>
-    <tableColumn id="6" name="[category]" dataDxfId="27"/>
-    <tableColumn id="7" name="[order]" dataDxfId="26"/>
-    <tableColumn id="13" name="[startingPool]" dataDxfId="25"/>
-    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="24"/>
-    <tableColumn id="16" name="[hidden]" dataDxfId="23"/>
-    <tableColumn id="15" name="[notInGatcha]" dataDxfId="22"/>
-    <tableColumn id="18" name="[associatedSeason]" dataDxfId="21"/>
-    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="20"/>
-    <tableColumn id="8" name="[gamePrefab]" dataDxfId="19"/>
-    <tableColumn id="9" name="[menuPrefab]" dataDxfId="18"/>
-    <tableColumn id="11" name="[icon]" dataDxfId="17"/>
-    <tableColumn id="4" name="[powerup]" dataDxfId="16"/>
-    <tableColumn id="20" name="[statPower]" dataDxfId="15"/>
-    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="14"/>
-    <tableColumn id="22" name="[sharedPower]" dataDxfId="13"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="12"/>
-    <tableColumn id="10" name="[tidDesc]" dataDxfId="11"/>
-    <tableColumn id="12" name="id" dataDxfId="10"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="29"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
+    <tableColumn id="3" name="[rarity]" dataDxfId="27"/>
+    <tableColumn id="6" name="[category]" dataDxfId="26"/>
+    <tableColumn id="7" name="[order]" dataDxfId="25"/>
+    <tableColumn id="13" name="[startingPool]" dataDxfId="24"/>
+    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="23"/>
+    <tableColumn id="16" name="[hidden]" dataDxfId="22"/>
+    <tableColumn id="15" name="[notInGatcha]" dataDxfId="21"/>
+    <tableColumn id="18" name="[associatedSeason]" dataDxfId="20"/>
+    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="19"/>
+    <tableColumn id="8" name="[gamePrefab]" dataDxfId="18"/>
+    <tableColumn id="9" name="[menuPrefab]" dataDxfId="17"/>
+    <tableColumn id="11" name="[icon]" dataDxfId="16"/>
+    <tableColumn id="4" name="[powerup]" dataDxfId="15"/>
+    <tableColumn id="20" name="[statPower]" dataDxfId="14"/>
+    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="13"/>
+    <tableColumn id="22" name="[sharedPower]" dataDxfId="12"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="11"/>
+    <tableColumn id="10" name="[tidDesc]" dataDxfId="10"/>
     <tableColumn id="17" name="[trackingName]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1776,8 +1963,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B12:G13" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="B12:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B19:G20" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B19:G20"/>
   <sortState ref="B95:F101">
     <sortCondition ref="D77:D84"/>
   </sortState>
@@ -2059,17 +2246,17 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:W22"/>
+  <dimension ref="B1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -2084,14 +2271,13 @@
     <col min="17" max="19" width="29.85546875" customWidth="1"/>
     <col min="20" max="20" width="23" customWidth="1"/>
     <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2106,100 +2292,97 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="23"/>
       <c r="P3" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="26" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="4" spans="2:23" ht="121.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" ht="121.5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="P4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>17</v>
+      <c r="V4" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="18" t="b">
         <v>0</v>
@@ -2215,60 +2398,57 @@
       </c>
       <c r="K5" s="18"/>
       <c r="L5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="R5" s="25" t="s">
+      <c r="S5" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="T5" s="11" t="s">
+      <c r="U5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5" s="11">
-        <v>0</v>
-      </c>
-      <c r="W5" s="18" t="s">
-        <v>38</v>
+      <c r="V5" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="18" t="b">
         <v>0</v>
@@ -2281,60 +2461,57 @@
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R6" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S6" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="V6" s="16">
-        <v>1</v>
-      </c>
-      <c r="W6" s="18" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="V6" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="18" t="b">
         <v>0</v>
@@ -2347,132 +2524,570 @@
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P7" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="R7" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="S7" s="25" t="s">
+      <c r="D8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="18">
+        <v>3</v>
+      </c>
+      <c r="G8" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="R8" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="S8" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="U8" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="V8" s="39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="18">
+        <v>4</v>
+      </c>
+      <c r="G9" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O9" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="R9" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="T9" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="U9" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="V9" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="18">
+        <v>5</v>
+      </c>
+      <c r="G10" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="O10" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q10" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="R10" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="S10" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="T10" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="U10" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="V10" s="45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="18">
+        <v>6</v>
+      </c>
+      <c r="G11" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="N11" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q11" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="R11" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="S11" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="T11" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="U11" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="V11" s="39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="18">
+        <v>7</v>
+      </c>
+      <c r="G12" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q12" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="R12" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="S12" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="V12" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="18">
+        <v>8</v>
+      </c>
+      <c r="G13" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q13" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="R13" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="S13" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U13" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="V13" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="18">
+        <v>9</v>
+      </c>
+      <c r="G14" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q14" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="R14" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="S14" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="U14" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="V14" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="2:14" ht="137.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="13">
+        <v>10</v>
+      </c>
+      <c r="E20" s="14">
+        <v>2</v>
+      </c>
+      <c r="F20" s="27">
+        <v>1</v>
+      </c>
+      <c r="G20" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="T7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="V7" s="11">
-        <v>2</v>
-      </c>
-      <c r="W7" s="18" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="9" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="28" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="28" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="12" spans="2:23" ht="137.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>33</v>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C28" s="28" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="13">
-        <v>10</v>
-      </c>
-      <c r="E13" s="14">
-        <v>2</v>
-      </c>
-      <c r="F13" s="27">
-        <v>1</v>
-      </c>
-      <c r="G13" s="27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="28" t="s">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C29" s="28" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="28" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E5:L7"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E5:L14"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tables updated with tids
Former-commit-id: a8bae9c795c212840c1c70f9c7f41a74f51f5e59
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="23540"/>
   </bookViews>
   <sheets>
     <sheet name="BabyDragons" sheetId="7" r:id="rId1"/>
@@ -2248,34 +2248,34 @@
   </sheetPr>
   <dimension ref="B1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.42578125" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" customWidth="1"/>
+    <col min="8" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.453125" customWidth="1"/>
+    <col min="13" max="13" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="29.81640625" customWidth="1"/>
     <col min="20" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:22" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="23"/>
@@ -2303,7 +2303,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="121.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" ht="119" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B8" s="29" t="s">
         <v>2</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B9" s="29" t="s">
         <v>2</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B10" s="40" t="s">
         <v>2</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B11" s="29" t="s">
         <v>2</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
         <v>2</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B13" s="21" t="s">
         <v>2</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
         <v>2</v>
       </c>
@@ -2998,8 +2998,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="2:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
@@ -3016,11 +3016,11 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:14" ht="137.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="134" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
         <v>2</v>
       </c>
@@ -3060,27 +3060,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C26" s="28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C27" s="28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C28" s="28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C29" s="28" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Excel and tables WIP
Former-commit-id: 4f6cb0dabc30e6e1348b5e23a1bc4c8658f5d153
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
   <si>
     <t>[sku]</t>
   </si>
@@ -484,6 +484,45 @@
       </rPr>
       <t xml:space="preserve"> firsts Flying pigs killed (with a Baby D. equipped) player doesn't get an 'extra' Gem, we will set prob. to 100% next time player kills a Flying pig, after that, prob. will be what was before. We need this value to 'show' player it is true they can get extra Gems and encourage them to get more Baby D.</t>
     </r>
+  </si>
+  <si>
+    <t>pet_baby_classic</t>
+  </si>
+  <si>
+    <t>pet_baby_crocodile</t>
+  </si>
+  <si>
+    <t>pet_baby_titan</t>
+  </si>
+  <si>
+    <t>pet_baby_jawfrey</t>
+  </si>
+  <si>
+    <t>pet_baby_dark</t>
+  </si>
+  <si>
+    <t>pet_baby_dino</t>
+  </si>
+  <si>
+    <t>pet_baby_alien</t>
+  </si>
+  <si>
+    <t>pet_baby_devil</t>
+  </si>
+  <si>
+    <t>pet_baby_tony</t>
+  </si>
+  <si>
+    <t>pet_baby_hedgehog</t>
+  </si>
+  <si>
+    <t>[tidDescription]</t>
+  </si>
+  <si>
+    <t>TID_SHARED_EXTRA_GEMS_NAME</t>
+  </si>
+  <si>
+    <t>TID_SHARED_EXTRA_GEMS_DESC</t>
   </si>
 </sst>
 </file>
@@ -911,7 +950,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <i val="0"/>
@@ -1945,51 +2064,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V14" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V14" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="B4:V14"/>
   <sortState ref="B5:T77">
     <sortCondition ref="D4:D77"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="3" name="[rarity]" dataDxfId="27"/>
-    <tableColumn id="6" name="[category]" dataDxfId="26"/>
-    <tableColumn id="7" name="[order]" dataDxfId="25"/>
-    <tableColumn id="13" name="[startingPool]" dataDxfId="24"/>
-    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="23"/>
-    <tableColumn id="16" name="[hidden]" dataDxfId="22"/>
-    <tableColumn id="15" name="[notInGatcha]" dataDxfId="21"/>
-    <tableColumn id="18" name="[associatedSeason]" dataDxfId="20"/>
-    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="19"/>
-    <tableColumn id="8" name="[gamePrefab]" dataDxfId="18"/>
-    <tableColumn id="9" name="[menuPrefab]" dataDxfId="17"/>
-    <tableColumn id="11" name="[icon]" dataDxfId="16"/>
-    <tableColumn id="4" name="[powerup]" dataDxfId="15"/>
-    <tableColumn id="20" name="[statPower]" dataDxfId="14"/>
-    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="13"/>
-    <tableColumn id="22" name="[sharedPower]" dataDxfId="12"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="2"/>
-    <tableColumn id="10" name="[tidDesc]" dataDxfId="0"/>
-    <tableColumn id="17" name="[trackingName]" dataDxfId="1"/>
+    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="31"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
+    <tableColumn id="3" name="[rarity]" dataDxfId="29"/>
+    <tableColumn id="6" name="[category]" dataDxfId="28"/>
+    <tableColumn id="7" name="[order]" dataDxfId="27"/>
+    <tableColumn id="13" name="[startingPool]" dataDxfId="26"/>
+    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="25"/>
+    <tableColumn id="16" name="[hidden]" dataDxfId="24"/>
+    <tableColumn id="15" name="[notInGatcha]" dataDxfId="23"/>
+    <tableColumn id="18" name="[associatedSeason]" dataDxfId="22"/>
+    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="21"/>
+    <tableColumn id="8" name="[gamePrefab]" dataDxfId="20"/>
+    <tableColumn id="9" name="[menuPrefab]" dataDxfId="19"/>
+    <tableColumn id="11" name="[icon]" dataDxfId="18"/>
+    <tableColumn id="4" name="[powerup]" dataDxfId="17"/>
+    <tableColumn id="20" name="[statPower]" dataDxfId="16"/>
+    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="15"/>
+    <tableColumn id="22" name="[sharedPower]" dataDxfId="14"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="4"/>
+    <tableColumn id="10" name="[tidDesc]" dataDxfId="2"/>
+    <tableColumn id="17" name="[trackingName]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B19:G20" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B19:G20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B19:I20" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="B19:I20"/>
   <sortState ref="B95:F101">
     <sortCondition ref="D77:D84"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="8"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="7"/>
-    <tableColumn id="3" name="[baseProbability]" dataDxfId="6"/>
-    <tableColumn id="4" name="[extraProbability]" dataDxfId="5"/>
-    <tableColumn id="5" name="[extraGems]" dataDxfId="4"/>
-    <tableColumn id="6" name="[firstSucceed]" dataDxfId="3"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="10"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
+    <tableColumn id="3" name="[baseProbability]" dataDxfId="8"/>
+    <tableColumn id="4" name="[extraProbability]" dataDxfId="7"/>
+    <tableColumn id="5" name="[extraGems]" dataDxfId="6"/>
+    <tableColumn id="6" name="[firstSucceed]" dataDxfId="5"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="1"/>
+    <tableColumn id="8" name="[tidDescription]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2263,8 +2384,8 @@
   </sheetPr>
   <dimension ref="B1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2422,7 +2543,7 @@
         <v>38</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="P5" s="15" t="s">
         <v>58</v>
@@ -2485,7 +2606,7 @@
         <v>47</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>57</v>
@@ -2548,7 +2669,7 @@
         <v>48</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="P7" s="15" t="s">
         <v>59</v>
@@ -2611,7 +2732,7 @@
         <v>74</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="P8" s="15" t="s">
         <v>104</v>
@@ -2674,7 +2795,7 @@
         <v>75</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>102</v>
@@ -2737,7 +2858,7 @@
         <v>76</v>
       </c>
       <c r="O10" s="33" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="P10" s="44" t="s">
         <v>106</v>
@@ -2800,7 +2921,7 @@
         <v>77</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="P11" s="34" t="s">
         <v>107</v>
@@ -2863,7 +2984,7 @@
         <v>78</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="P12" s="15" t="s">
         <v>109</v>
@@ -2926,7 +3047,7 @@
         <v>79</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="P13" s="15" t="s">
         <v>111</v>
@@ -2989,7 +3110,7 @@
         <v>80</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="P14" s="15" t="s">
         <v>113</v>
@@ -3054,6 +3175,12 @@
       <c r="G19" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="H19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
@@ -3073,6 +3200,12 @@
       </c>
       <c r="G20" s="26">
         <v>4</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Baby Dragons: Content - Added missing xml. Shared Powers: Content - Added "icon" column. Renamed "tidDescription" to "tidDesc" to be consistent with power definitions table.
Former-commit-id: 4eef55beeebf80936f5408f6ffaffff0d6d907e0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123A3AE7-7614-4121-8BFF-5891A7942F3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BabyDragons" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="129">
   <si>
     <t>[sku]</t>
   </si>
@@ -516,19 +523,19 @@
     <t>pet_baby_hedgehog</t>
   </si>
   <si>
-    <t>[tidDescription]</t>
-  </si>
-  <si>
     <t>TID_SHARED_EXTRA_GEMS_NAME</t>
   </si>
   <si>
     <t>TID_SHARED_EXTRA_GEMS_DESC</t>
+  </si>
+  <si>
+    <t>icon_power_baby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -803,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -842,9 +849,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -874,9 +878,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -945,12 +946,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="38">
     <dxf>
       <font>
         <b val="0"/>
@@ -970,10 +974,60 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1013,7 +1067,107 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1029,6 +1183,142 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1067,34 +1357,6 @@
     </dxf>
     <dxf>
       <font>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1128,205 +1390,6 @@
         </top>
         <bottom style="thin">
           <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -2064,53 +2127,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V14" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
-  <autoFilter ref="B4:V14"/>
-  <sortState ref="B5:T77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V14" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B4:V14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:T77">
     <sortCondition ref="D4:D77"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="{babyDragonDefinitions}" dataDxfId="31"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
-    <tableColumn id="3" name="[rarity]" dataDxfId="29"/>
-    <tableColumn id="6" name="[category]" dataDxfId="28"/>
-    <tableColumn id="7" name="[order]" dataDxfId="27"/>
-    <tableColumn id="13" name="[startingPool]" dataDxfId="26"/>
-    <tableColumn id="14" name="[loadingTeasing]" dataDxfId="25"/>
-    <tableColumn id="16" name="[hidden]" dataDxfId="24"/>
-    <tableColumn id="15" name="[notInGatcha]" dataDxfId="23"/>
-    <tableColumn id="18" name="[associatedSeason]" dataDxfId="22"/>
-    <tableColumn id="19" name="[tidUnlockCondition]" dataDxfId="21"/>
-    <tableColumn id="8" name="[gamePrefab]" dataDxfId="20"/>
-    <tableColumn id="9" name="[menuPrefab]" dataDxfId="19"/>
-    <tableColumn id="11" name="[icon]" dataDxfId="18"/>
-    <tableColumn id="4" name="[powerup]" dataDxfId="17"/>
-    <tableColumn id="20" name="[statPower]" dataDxfId="16"/>
-    <tableColumn id="21" name="[motherDragonSKU]" dataDxfId="15"/>
-    <tableColumn id="22" name="[sharedPower]" dataDxfId="14"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="4"/>
-    <tableColumn id="10" name="[tidDesc]" dataDxfId="2"/>
-    <tableColumn id="17" name="[trackingName]" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{babyDragonDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[rarity]" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[category]" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[startingPool]" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[loadingTeasing]" dataDxfId="26"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[hidden]" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[notInGatcha]" dataDxfId="24"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[associatedSeason]" dataDxfId="23"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[tidUnlockCondition]" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[gamePrefab]" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[menuPrefab]" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[icon]" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[powerup]" dataDxfId="18"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[statPower]" dataDxfId="17"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[motherDragonSKU]" dataDxfId="16"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[sharedPower]" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[tidName]" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tidDesc]" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[trackingName]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B19:I20" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="B19:I20"/>
-  <sortState ref="B95:F101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B19:J20" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="B19:J20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B95:F101">
     <sortCondition ref="D77:D84"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" name="{sharedPowerupDefinitions}" dataDxfId="10"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
-    <tableColumn id="3" name="[baseProbability]" dataDxfId="8"/>
-    <tableColumn id="4" name="[extraProbability]" dataDxfId="7"/>
-    <tableColumn id="5" name="[extraGems]" dataDxfId="6"/>
-    <tableColumn id="6" name="[firstSucceed]" dataDxfId="5"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="1"/>
-    <tableColumn id="8" name="[tidDescription]" dataDxfId="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{sharedPowerupDefinitions}" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[baseProbability]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[extraProbability]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[extraGems]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[firstSucceed]" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{6570B788-C4AD-4AFB-B1BB-102A681AF16D}" name="[icon]" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[tidDesc]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2378,13 +2442,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="B1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -2431,11 +2495,11 @@
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="22"/>
-      <c r="P3" s="25" t="s">
+      <c r="D3" s="21"/>
+      <c r="P3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="25" t="s">
+      <c r="Q3" s="24" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2485,19 +2549,19 @@
       <c r="P4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="22" t="s">
         <v>42</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="45" t="s">
+      <c r="U4" s="43" t="s">
         <v>7</v>
       </c>
       <c r="V4" s="4" t="s">
@@ -2505,35 +2569,35 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="17">
-        <v>0</v>
-      </c>
-      <c r="G5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17" t="s">
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="8" t="s">
@@ -2545,58 +2609,58 @@
       <c r="O5" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="P5" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="Q5" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="R5" s="24" t="s">
+      <c r="R5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="S5" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="U5" s="46" t="s">
+      <c r="U5" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="V5" s="17" t="s">
+      <c r="V5" s="16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <v>1</v>
       </c>
-      <c r="G6" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17" t="s">
+      <c r="G6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16" t="s">
         <v>36</v>
       </c>
       <c r="M6" s="8" t="s">
@@ -2608,58 +2672,58 @@
       <c r="O6" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" s="24" t="s">
+      <c r="Q6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="R6" s="24" t="s">
+      <c r="R6" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="S6" s="24" t="s">
+      <c r="S6" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="46" t="s">
+      <c r="U6" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="V6" s="17" t="s">
+      <c r="V6" s="16" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>2</v>
       </c>
-      <c r="G7" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17" t="s">
+      <c r="G7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="8" t="s">
@@ -2671,310 +2735,310 @@
       <c r="O7" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="24" t="s">
+      <c r="Q7" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="R7" s="24" t="s">
+      <c r="R7" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="S7" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="U7" s="47" t="s">
+      <c r="U7" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="V7" s="17" t="s">
+      <c r="V7" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>3</v>
       </c>
-      <c r="G8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31" t="s">
+      <c r="G8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="O8" s="33" t="s">
+      <c r="O8" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="P8" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="R8" s="35" t="s">
+      <c r="R8" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="S8" s="35" t="s">
+      <c r="S8" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="36" t="s">
+      <c r="T8" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="U8" s="48" t="s">
+      <c r="U8" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="V8" s="37" t="s">
+      <c r="V8" s="35" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <v>4</v>
       </c>
-      <c r="G9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31" t="s">
+      <c r="G9" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="O9" s="33" t="s">
+      <c r="O9" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="P9" s="15" t="s">
+      <c r="P9" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Q9" s="24" t="s">
+      <c r="Q9" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="R9" s="35" t="s">
+      <c r="R9" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="S9" s="35" t="s">
+      <c r="S9" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="T9" s="36" t="s">
+      <c r="T9" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="U9" s="48" t="s">
+      <c r="U9" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="V9" s="37" t="s">
+      <c r="V9" s="35" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="16">
         <v>5</v>
       </c>
-      <c r="G10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30" t="s">
+      <c r="G10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M10" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="N10" s="33" t="s">
+      <c r="N10" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="O10" s="33" t="s">
+      <c r="O10" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="P10" s="44" t="s">
+      <c r="P10" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="Q10" s="43" t="s">
+      <c r="Q10" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="R10" s="40" t="s">
+      <c r="R10" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="S10" s="40" t="s">
+      <c r="S10" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="T10" s="41" t="s">
+      <c r="T10" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="U10" s="49" t="s">
+      <c r="U10" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="V10" s="42" t="s">
+      <c r="V10" s="40" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <v>6</v>
       </c>
-      <c r="G11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31" t="s">
+      <c r="G11" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M11" s="32" t="s">
+      <c r="M11" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="32" t="s">
+      <c r="N11" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="O11" s="33" t="s">
+      <c r="O11" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="P11" s="34" t="s">
+      <c r="P11" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="Q11" s="35" t="s">
+      <c r="Q11" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="R11" s="35" t="s">
+      <c r="R11" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="S11" s="35" t="s">
+      <c r="S11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="T11" s="36" t="s">
+      <c r="T11" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="U11" s="48" t="s">
+      <c r="U11" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="V11" s="37" t="s">
+      <c r="V11" s="35" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <v>7</v>
       </c>
-      <c r="G12" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17" t="s">
+      <c r="G12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
         <v>36</v>
       </c>
       <c r="M12" s="8" t="s">
@@ -2986,58 +3050,58 @@
       <c r="O12" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="P12" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="Q12" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="R12" s="24" t="s">
+      <c r="R12" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="S12" s="24" t="s">
+      <c r="S12" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="U12" s="46" t="s">
+      <c r="U12" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="V12" s="17" t="s">
+      <c r="V12" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <v>8</v>
       </c>
-      <c r="G13" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17" t="s">
+      <c r="G13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16" t="s">
         <v>36</v>
       </c>
       <c r="M13" s="8" t="s">
@@ -3049,58 +3113,58 @@
       <c r="O13" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="P13" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="R13" s="24" t="s">
+      <c r="R13" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="S13" s="24" t="s">
+      <c r="S13" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="U13" s="46" t="s">
+      <c r="U13" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="V13" s="17" t="s">
+      <c r="V13" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="16">
         <v>9</v>
       </c>
-      <c r="G14" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17" t="s">
+      <c r="G14" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16" t="s">
         <v>36</v>
       </c>
       <c r="M14" s="8" t="s">
@@ -3112,25 +3176,25 @@
       <c r="O14" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="P14" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="Q14" s="24" t="s">
+      <c r="Q14" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="R14" s="24" t="s">
+      <c r="R14" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="S14" s="24" t="s">
+      <c r="S14" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T14" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="U14" s="47" t="s">
+      <c r="U14" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="V14" s="17" t="s">
+      <c r="V14" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3166,46 +3230,52 @@
       <c r="D19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="9" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>126</v>
+      <c r="J19" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="13">
         <v>5</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <v>2</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="13">
         <v>1</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="13">
         <v>4</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="J20" s="48" t="s">
         <v>127</v>
-      </c>
-      <c r="I20" s="26" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -3214,28 +3284,28 @@
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="25" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="25" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="25" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E5:L14"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E5:L14" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Baby Pets: Development - Properly implemented text colors, replacements and power icons.
Former-commit-id: 7f0a65653ab9d3f4b5ec6439e1424d862f62bcc8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123A3AE7-7614-4121-8BFF-5891A7942F3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A56ECD5-4B01-4987-ABCF-95622F4B03DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BabyDragons" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="131">
   <si>
     <t>[sku]</t>
   </si>
@@ -529,7 +529,13 @@
     <t>TID_SHARED_EXTRA_GEMS_DESC</t>
   </si>
   <si>
-    <t>icon_power_baby</t>
+    <t>[type]</t>
+  </si>
+  <si>
+    <t>collection</t>
+  </si>
+  <si>
+    <t>icon_power_baby_collection</t>
   </si>
 </sst>
 </file>
@@ -954,7 +960,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="39">
     <dxf>
       <font>
         <b val="0"/>
@@ -969,6 +975,162 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1043,121 +1205,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2127,54 +2174,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V14" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="petDefinitions2" displayName="petDefinitions2" ref="B4:V14" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B4:V14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:T77">
     <sortCondition ref="D4:D77"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{babyDragonDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[rarity]" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[category]" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="28"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[startingPool]" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[loadingTeasing]" dataDxfId="26"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[hidden]" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[notInGatcha]" dataDxfId="24"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[associatedSeason]" dataDxfId="23"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[tidUnlockCondition]" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[gamePrefab]" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[menuPrefab]" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[icon]" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[powerup]" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[statPower]" dataDxfId="17"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[motherDragonSKU]" dataDxfId="16"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[sharedPower]" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[tidName]" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tidDesc]" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[trackingName]" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{babyDragonDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[rarity]" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[category]" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[order]" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[startingPool]" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[loadingTeasing]" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[hidden]" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[notInGatcha]" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[associatedSeason]" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[tidUnlockCondition]" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[gamePrefab]" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[menuPrefab]" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[icon]" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[powerup]" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[statPower]" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[motherDragonSKU]" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[sharedPower]" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[tidName]" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tidDesc]" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[trackingName]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B19:J20" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B19:J20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B95:F101">
-    <sortCondition ref="D77:D84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="petCategoryDefinitions3" displayName="petCategoryDefinitions3" ref="B19:K20" totalsRowShown="0" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="B19:K20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B95:G101">
+    <sortCondition ref="E77:E84"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{sharedPowerupDefinitions}" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[baseProbability]" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[extraProbability]" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[extraGems]" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[firstSucceed]" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{6570B788-C4AD-4AFB-B1BB-102A681AF16D}" name="[icon]" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[tidDesc]" dataDxfId="3"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{sharedPowerupDefinitions}" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{EF0D6C29-320C-44D2-B2FA-653E99769602}" name="[type]" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[baseProbability]" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[extraProbability]" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[extraGems]" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[firstSucceed]" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{6570B788-C4AD-4AFB-B1BB-102A681AF16D}" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[tidDesc]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2449,7 +2497,7 @@
   <dimension ref="B1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3227,25 +3275,28 @@
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="J19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="K19" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3256,25 +3307,28 @@
       <c r="C20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="13">
         <v>5</v>
       </c>
-      <c r="E20" s="13">
+      <c r="F20" s="13">
         <v>2</v>
       </c>
-      <c r="F20" s="13">
+      <c r="G20" s="13">
         <v>1</v>
       </c>
-      <c r="G20" s="13">
+      <c r="H20" s="13">
         <v>4</v>
       </c>
-      <c r="H20" s="48" t="s">
-        <v>128</v>
-      </c>
       <c r="I20" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="J20" s="48" t="s">
+      <c r="K20" s="48" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Baby Dragons: Fix - Baby Tony didn't have the right mother dragon sku.
Former-commit-id: 0442af74010bbad614ce8cbdb593d2d4883bea77
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_BabyDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_BabyDragons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A56ECD5-4B01-4987-ABCF-95622F4B03DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0ADDAE-843C-47B5-A605-5A059861F465}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,9 +347,6 @@
     <t>dragon_devil</t>
   </si>
   <si>
-    <t>dragon_tony</t>
-  </si>
-  <si>
     <t>dragon_hedgehog</t>
   </si>
   <si>
@@ -536,6 +533,9 @@
   </si>
   <si>
     <t>icon_power_baby_collection</t>
+  </si>
+  <si>
+    <t>dragon_fat</t>
   </si>
 </sst>
 </file>
@@ -975,17 +975,16 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -998,8 +997,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1054,6 +1051,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1092,17 +1090,16 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1115,6 +1112,83 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1131,87 +1205,13 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2215,14 +2215,14 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{sharedPowerupDefinitions}" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{EF0D6C29-320C-44D2-B2FA-653E99769602}" name="[type]" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[baseProbability]" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[extraProbability]" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[extraGems]" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[firstSucceed]" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{6570B788-C4AD-4AFB-B1BB-102A681AF16D}" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[tidDesc]" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{EF0D6C29-320C-44D2-B2FA-653E99769602}" name="[type]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[baseProbability]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[extraProbability]" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[extraGems]" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[firstSucceed]" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6570B788-C4AD-4AFB-B1BB-102A681AF16D}" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[tidDesc]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2496,8 +2496,8 @@
   </sheetPr>
   <dimension ref="B1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +2655,7 @@
         <v>38</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P5" s="14" t="s">
         <v>58</v>
@@ -2718,7 +2718,7 @@
         <v>47</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P6" s="14" t="s">
         <v>57</v>
@@ -2781,7 +2781,7 @@
         <v>48</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P7" s="14" t="s">
         <v>59</v>
@@ -2844,13 +2844,13 @@
         <v>74</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R8" s="33" t="s">
         <v>81</v>
@@ -2859,10 +2859,10 @@
         <v>27</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U8" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V8" s="35" t="s">
         <v>60</v>
@@ -2907,13 +2907,13 @@
         <v>75</v>
       </c>
       <c r="O9" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P9" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q9" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="Q9" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="R9" s="33" t="s">
         <v>82</v>
@@ -2922,10 +2922,10 @@
         <v>27</v>
       </c>
       <c r="T9" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U9" s="46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V9" s="35" t="s">
         <v>61</v>
@@ -2970,13 +2970,13 @@
         <v>76</v>
       </c>
       <c r="O10" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P10" s="42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q10" s="41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R10" s="38" t="s">
         <v>83</v>
@@ -2985,10 +2985,10 @@
         <v>27</v>
       </c>
       <c r="T10" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U10" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V10" s="40" t="s">
         <v>62</v>
@@ -3033,13 +3033,13 @@
         <v>77</v>
       </c>
       <c r="O11" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P11" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q11" s="33" t="s">
         <v>107</v>
-      </c>
-      <c r="Q11" s="33" t="s">
-        <v>108</v>
       </c>
       <c r="R11" s="33" t="s">
         <v>84</v>
@@ -3048,10 +3048,10 @@
         <v>27</v>
       </c>
       <c r="T11" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U11" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V11" s="35" t="s">
         <v>63</v>
@@ -3096,13 +3096,13 @@
         <v>78</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P12" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="23" t="s">
         <v>109</v>
-      </c>
-      <c r="Q12" s="23" t="s">
-        <v>110</v>
       </c>
       <c r="R12" s="23" t="s">
         <v>85</v>
@@ -3111,10 +3111,10 @@
         <v>27</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U12" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V12" s="16" t="s">
         <v>64</v>
@@ -3159,25 +3159,25 @@
         <v>79</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T13" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U13" s="44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V13" s="16" t="s">
         <v>65</v>
@@ -3222,25 +3222,25 @@
         <v>80</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S14" s="23" t="s">
         <v>27</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U14" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V14" s="16" t="s">
         <v>66</v>
@@ -3276,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>29</v>
@@ -3308,7 +3308,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20" s="13">
         <v>5</v>
@@ -3323,13 +3323,13 @@
         <v>4</v>
       </c>
       <c r="I20" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J20" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="K20" s="48" t="s">
         <v>126</v>
-      </c>
-      <c r="K20" s="48" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -3339,7 +3339,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C26" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
@@ -3354,7 +3354,7 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C29" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>